<commit_message>
add comment for excel template
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/files/reimburseprice_template.xlsx
+++ b/src/main/webapp/resources/files/reimburseprice_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>TMTID</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>TMTID และ EFFECTIVE_DATE ห้ามเป็นค่าว่าง</t>
+  </si>
+  <si>
+    <t>PRICE ไม่ต้องใส่หน่วย</t>
   </si>
 </sst>
 </file>
@@ -371,7 +374,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -415,6 +418,9 @@
       <c r="C3">
         <v>20.5</v>
       </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">

</xml_diff>